<commit_message>
Functions DI and AutoMapper Update Employer excel data Remove QueueStorageConnectionString
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.FileReader.Excel.IntegrationTests/Employer/Employer-Simple.xlsx
+++ b/src/Sfa.Tl.Matching.FileReader.Excel.IntegrationTests/Employer/Employer-Simple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Esfa\das-poc-matching\sfa.poc.matching.fileupload\Esfa.Poc.Matching.Application.IntegrationTests\Employers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Esfa\tl-matching\src\Sfa.Tl.Matching.FileReader.Excel.IntegrationTests\Employer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B6D6AC-4850-4EB7-996B-2436D2CDCF5F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE05324-43CE-4A99-8A02-FE065F00ABEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>(Do Not Modify) Account</t>
   </si>
@@ -41,9 +41,6 @@
     <t>AUPA</t>
   </si>
   <si>
-    <t>Company Type</t>
-  </si>
-  <si>
     <t>Primary Contact</t>
   </si>
   <si>
@@ -53,33 +50,9 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>Address 1: City</t>
-  </si>
-  <si>
-    <t>Address 1: Country/Region</t>
-  </si>
-  <si>
     <t>Post Code</t>
   </si>
   <si>
-    <t>Created By</t>
-  </si>
-  <si>
-    <t>Created On</t>
-  </si>
-  <si>
-    <t>Modified By</t>
-  </si>
-  <si>
-    <t>Modified On</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -120,18 +93,6 @@
   </si>
   <si>
     <t>Checksum</t>
-  </si>
-  <si>
-    <t>www.website.com</t>
-  </si>
-  <si>
-    <t>Address1</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Region</t>
   </si>
   <si>
     <t>S1 1AA</t>
@@ -177,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -187,19 +148,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -221,28 +171,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T2" totalsRowShown="0">
-  <autoFilter ref="A1:T2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K2" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Account"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(Do Not Modify) Modified On"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Company Name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Also Known As"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="AUPA"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Company Type"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Primary Contact"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Main Phone"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Email" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Website"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Address 1"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Address 1: City"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Address 1: Country/Region"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Post Code"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Created By"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Created On"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Modified By"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Modified On"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Owner"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -547,10 +488,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -561,23 +502,14 @@
     <col min="4" max="4" width="42" style="4" customWidth="1"/>
     <col min="5" max="5" width="14" style="5" customWidth="1"/>
     <col min="6" max="6" width="14" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14" style="7" customWidth="1"/>
-    <col min="8" max="8" width="21" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14" style="8" customWidth="1"/>
     <col min="9" max="9" width="14" style="9" customWidth="1"/>
     <col min="10" max="10" width="14" style="10" customWidth="1"/>
     <col min="11" max="11" width="14" style="11" customWidth="1"/>
-    <col min="12" max="12" width="14" style="12" customWidth="1"/>
-    <col min="13" max="13" width="14" style="13" customWidth="1"/>
-    <col min="14" max="14" width="14" style="14" customWidth="1"/>
-    <col min="15" max="15" width="14" style="15" customWidth="1"/>
-    <col min="16" max="16" width="14" style="16" customWidth="1"/>
-    <col min="17" max="17" width="14" style="17" customWidth="1"/>
-    <col min="18" max="18" width="14" style="18" customWidth="1"/>
-    <col min="19" max="19" width="14" style="19" customWidth="1"/>
-    <col min="20" max="20" width="14" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,98 +543,44 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>32</v>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="C2" s="3">
         <v>43439.620694444398</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="20">
+        <v>12</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="11">
         <v>7777744465</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="17">
-        <v>43439.615983796299</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="19">
-        <v>43439.620694444398</v>
-      </c>
-      <c r="T2" s="20" t="s">
-        <v>19</v>
+      <c r="I2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
+  <dataValidations count="8">
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="(Do Not Modify) Modified On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -712,37 +590,20 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 100 characters long." promptTitle="Text" prompt="Maximum Length: 100 characters." sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This Primary Contact record must already exist in Microsoft Dynamics CRM or in this source file." sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 55 characters long." promptTitle="Text" prompt="Maximum Length: 55 characters." sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This Primary Contact record must already exist in Microsoft Dynamics CRM or in this source file." sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 55 characters long." promptTitle="Text" prompt="Maximum Length: 55 characters." sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>55</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 159 characters long." promptTitle="Text" prompt="Maximum Length: 159 characters." sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 159 characters long." promptTitle="Text" prompt="Maximum Length: 159 characters." sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>159</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 200 characters long." promptTitle="Text" prompt="Maximum Length: 200 characters." sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>200</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 1000 characters long." promptTitle="Text" prompt="Maximum Length: 1000 characters." sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0000-000009000000}">
-      <formula1>1000</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 80 characters long." promptTitle="Text" prompt="Maximum Length: 80 characters." sqref="M2:N1048576" xr:uid="{00000000-0002-0000-0000-00000A000000}">
-      <formula1>80</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 8 characters long." promptTitle="Text (required)" prompt="Maximum Length: 8 characters." sqref="O2:O1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 8 characters long." promptTitle="Text (required)" prompt="Maximum Length: 8 characters." sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>8</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This Created By record must already exist in Microsoft Dynamics CRM or in this source file." sqref="P2:P1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="Created On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="Q2:Q1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}">
-      <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This Modified By record must already exist in Microsoft Dynamics CRM or in this source file." sqref="R2:R1048576" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="Modified On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="S2:S1048576" xr:uid="{00000000-0002-0000-0000-000010000000}">
-      <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics CRM or in this source file." sqref="T2:T1048576" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics CRM or in this source file." sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{7A3CD807-0926-4B9D-8950-B6D78E3B1357}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{7A3CD807-0926-4B9D-8950-B6D78E3B1357}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -751,18 +612,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="AUPA must be selected from the drop-down list." promptTitle="Option set" prompt="Select a value from the drop-down list." xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>hiddenSheet!$A$2:$D$2</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="Company Type must be selected from the drop-down list." promptTitle="Option set" prompt="Select a value from the drop-down list." xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>hiddenSheet!$A$3:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -781,41 +636,41 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>